<commit_message>
added images and matrices to assignment sheet Signed-off-by: RobSmyth23 <145557344+RobSmyth23@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Assignment 1.xlsx
+++ b/Assignment 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StudentRobertSmyth(T\Desktop\My_Initial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robsm\Desktop\CGAss1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2FC840-AA18-4355-BE02-51A1D9B0DE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{173FADCC-A322-43FC-965D-32524C73F018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment generation" sheetId="1" r:id="rId1"/>
@@ -418,83 +418,83 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -518,52 +518,43 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -668,6 +659,314 @@
         <a:xfrm>
           <a:off x="1815353" y="313766"/>
           <a:ext cx="3546931" cy="1725706"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>22300</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>305614</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15EEE331-DA7F-DDE7-FCD0-4C4E894AF861}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1836964" y="8028214"/>
+          <a:ext cx="3791479" cy="5830114"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1135343</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>438982</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2341CDE-9F61-8B49-1D4F-1FF2A4A71FD5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1836964" y="15063107"/>
+          <a:ext cx="3639058" cy="5963482"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>312964</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>861539</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F1A3E6D-7978-37E5-22EA-0C351B8EF15F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8191501" y="13865678"/>
+          <a:ext cx="2735036" cy="548575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>146142</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>315140</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28EBCF92-9B93-DBBA-F05B-386BB2C18047}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1836964" y="22274893"/>
+          <a:ext cx="3915321" cy="5839640"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>275561</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>4299857</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC501FAE-2DDC-32F8-C66E-53B8BCAE5204}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8191500" y="22274893"/>
+          <a:ext cx="3010597" cy="4299857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>435429</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1106751</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>1121325</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A10F6187-3937-BBE6-37BC-7AAFFD299625}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1932214" y="30003750"/>
+          <a:ext cx="3515216" cy="685896"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>435429</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>408215</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>751508</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>1113163</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E5BD23C-84F3-0264-4F2F-1C46679D795D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2272393" y="35501036"/>
+          <a:ext cx="2819794" cy="704948"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -983,24 +1282,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
       <c r="K2" s="28" t="s">
         <v>35</v>
       </c>
@@ -1198,8 +1497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:E15"/>
+    <sheetView topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1223,10 +1522,10 @@
     </row>
     <row r="2" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="5"/>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="47"/>
+      <c r="E2" s="38"/>
       <c r="F2" s="8"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -1237,15 +1536,15 @@
     </row>
     <row r="3" spans="3:13" ht="408.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="5"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="33"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="6"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="33"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="6"/>
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
-      <c r="L3" s="34"/>
+      <c r="L3" s="7"/>
       <c r="M3" s="12"/>
     </row>
     <row r="4" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1258,10 +1557,10 @@
     </row>
     <row r="5" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="5"/>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="47"/>
+      <c r="E5" s="38"/>
       <c r="F5" s="8"/>
       <c r="H5" s="15"/>
       <c r="I5" s="12"/>
@@ -1270,8 +1569,8 @@
     </row>
     <row r="6" spans="3:13" ht="138.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="5"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="40"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="36"/>
       <c r="F6" s="16"/>
       <c r="G6" s="12"/>
       <c r="H6" s="15"/>
@@ -1282,7 +1581,7 @@
     <row r="7" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D7" s="13"/>
       <c r="E7" s="14"/>
-      <c r="F7" s="35"/>
+      <c r="F7" s="15"/>
       <c r="G7" s="12"/>
       <c r="H7" s="15"/>
       <c r="I7" s="12"/>
@@ -1291,10 +1590,10 @@
     </row>
     <row r="8" spans="3:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="5"/>
-      <c r="D8" s="46" t="s">
+      <c r="D8" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="47"/>
+      <c r="E8" s="38"/>
       <c r="F8" s="17"/>
       <c r="G8" s="12"/>
       <c r="H8" s="15"/>
@@ -1304,8 +1603,8 @@
     </row>
     <row r="9" spans="3:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="5"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="40"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="36"/>
       <c r="F9" s="17"/>
       <c r="G9" s="12"/>
       <c r="H9" s="15"/>
@@ -1325,28 +1624,28 @@
     </row>
     <row r="11" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="5"/>
-      <c r="D11" s="46" t="s">
+      <c r="D11" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="47"/>
+      <c r="E11" s="38"/>
       <c r="F11" s="18"/>
       <c r="G11" s="19"/>
-      <c r="H11" s="44" t="s">
+      <c r="H11" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="45"/>
+      <c r="I11" s="40"/>
       <c r="J11" s="8"/>
       <c r="L11" s="15"/>
       <c r="M11" s="12"/>
     </row>
     <row r="12" spans="3:13" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="5"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="40"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="36"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="40"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="36"/>
       <c r="J12" s="16"/>
       <c r="K12" s="12"/>
       <c r="L12" s="15"/>
@@ -1366,10 +1665,10 @@
     </row>
     <row r="14" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="5"/>
-      <c r="D14" s="46" t="s">
+      <c r="D14" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="47"/>
+      <c r="E14" s="38"/>
       <c r="F14" s="17"/>
       <c r="G14" s="12"/>
       <c r="H14" s="15"/>
@@ -1381,8 +1680,8 @@
     </row>
     <row r="15" spans="3:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="5"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="40"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="36"/>
       <c r="F15" s="17"/>
       <c r="G15" s="12"/>
       <c r="H15" s="15"/>
@@ -1406,10 +1705,10 @@
     </row>
     <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="5"/>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="47"/>
+      <c r="E17" s="38"/>
       <c r="F17" s="18"/>
       <c r="G17" s="12"/>
       <c r="H17" s="15"/>
@@ -1421,8 +1720,8 @@
     </row>
     <row r="18" spans="1:13" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18" s="5"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="40"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="36"/>
       <c r="F18" s="20"/>
       <c r="H18" s="15"/>
       <c r="I18" s="12"/>
@@ -1443,18 +1742,18 @@
     </row>
     <row r="20" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" s="5"/>
-      <c r="D20" s="46" t="s">
+      <c r="D20" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="47"/>
+      <c r="E20" s="38"/>
       <c r="F20" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="43"/>
-      <c r="H20" s="44" t="s">
+      <c r="G20" s="42"/>
+      <c r="H20" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="I20" s="45"/>
+      <c r="I20" s="40"/>
       <c r="J20" s="17"/>
       <c r="K20" s="12"/>
       <c r="L20" s="15"/>
@@ -1462,12 +1761,12 @@
     </row>
     <row r="21" spans="1:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" s="5"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="40"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="36"/>
       <c r="F21" s="41"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="40"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="36"/>
       <c r="J21" s="17"/>
       <c r="K21" s="12"/>
       <c r="L21" s="15"/>
@@ -1485,33 +1784,33 @@
     </row>
     <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" s="5"/>
-      <c r="D23" s="46" t="s">
+      <c r="D23" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="47"/>
+      <c r="E23" s="38"/>
       <c r="F23" s="9"/>
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
       <c r="I23" s="22"/>
       <c r="J23" s="10"/>
       <c r="K23" s="18"/>
-      <c r="L23" s="44" t="s">
+      <c r="L23" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="M23" s="45"/>
+      <c r="M23" s="40"/>
     </row>
     <row r="24" spans="1:13" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" s="5"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="40"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="36"/>
       <c r="F24" s="6"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
       <c r="J24" s="7"/>
       <c r="K24" s="23"/>
-      <c r="L24" s="38"/>
-      <c r="M24" s="40"/>
+      <c r="L24" s="35"/>
+      <c r="M24" s="36"/>
     </row>
     <row r="25" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D25" s="13"/>
@@ -1524,10 +1823,10 @@
     <row r="26" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="4"/>
       <c r="C26" s="24"/>
-      <c r="D26" s="44" t="s">
+      <c r="D26" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="45"/>
+      <c r="E26" s="40"/>
       <c r="F26" s="12"/>
       <c r="J26" s="15"/>
       <c r="K26" s="12"/>
@@ -1538,8 +1837,8 @@
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="40"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="36"/>
       <c r="F27" s="12"/>
       <c r="J27" s="15"/>
       <c r="K27" s="12"/>
@@ -1557,15 +1856,15 @@
       <c r="M28" s="12"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="45"/>
+      <c r="B29" s="40"/>
       <c r="C29" s="25"/>
-      <c r="D29" s="46" t="s">
+      <c r="D29" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="47"/>
+      <c r="E29" s="38"/>
       <c r="F29" s="9"/>
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
@@ -1576,11 +1875,11 @@
       <c r="M29" s="12"/>
     </row>
     <row r="30" spans="1:13" ht="322.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="38"/>
-      <c r="B30" s="40"/>
+      <c r="A30" s="35"/>
+      <c r="B30" s="36"/>
       <c r="C30" s="25"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="40"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="36"/>
       <c r="F30" s="20"/>
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
@@ -1598,44 +1897,44 @@
       <c r="M31" s="8"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="46" t="s">
+      <c r="A32" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="47"/>
+      <c r="B32" s="38"/>
       <c r="C32" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="46" t="s">
+      <c r="D32" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="47"/>
+      <c r="E32" s="38"/>
       <c r="F32" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="G32" s="42"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="42"/>
-      <c r="J32" s="42"/>
-      <c r="K32" s="43"/>
-      <c r="L32" s="46" t="s">
+      <c r="G32" s="44"/>
+      <c r="H32" s="44"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="44"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="M32" s="47"/>
+      <c r="M32" s="38"/>
     </row>
     <row r="33" spans="1:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="48"/>
-      <c r="B33" s="39"/>
+      <c r="A33" s="45"/>
+      <c r="B33" s="43"/>
       <c r="C33" s="17"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="40"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="36"/>
       <c r="F33" s="41"/>
-      <c r="G33" s="42"/>
-      <c r="H33" s="42"/>
-      <c r="I33" s="42"/>
-      <c r="J33" s="42"/>
-      <c r="K33" s="43"/>
-      <c r="L33" s="38"/>
-      <c r="M33" s="39"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="42"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="43"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="21"/>
@@ -1647,33 +1946,46 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C35" s="5"/>
-      <c r="D35" s="44" t="s">
+      <c r="D35" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="E35" s="45"/>
+      <c r="E35" s="40"/>
       <c r="F35" s="12"/>
     </row>
     <row r="36" spans="1:13" ht="213.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="5"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="40"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="36"/>
       <c r="F36" s="12"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E38" s="26"/>
       <c r="F38" s="26"/>
-      <c r="H38" s="38"/>
-      <c r="I38" s="39"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="43"/>
     </row>
     <row r="91" ht="0.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F32:K32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:K33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="L33:M33"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="H11:I11"/>
@@ -1690,25 +2002,12 @@
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D23:E23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F32:K32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:K33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>